<commit_message>
fixed the date output in the procurement insert
</commit_message>
<xml_diff>
--- a/public/test.xlsx
+++ b/public/test.xlsx
@@ -374,7 +374,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="SheetJS"/>
-  <dimension ref="A1:AL3"/>
+  <dimension ref="A1:AL2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -390,13 +390,13 @@
         <v/>
       </c>
       <c r="D1" s="1" t="str">
-        <v>TEST DATA</v>
+        <v>Flood</v>
       </c>
       <c r="E1" s="1" t="str">
         <v/>
       </c>
       <c r="F1" s="1" t="str">
-        <v/>
+        <v>Agency to Agency</v>
       </c>
       <c r="G1" s="1" t="str">
         <v/>
@@ -435,13 +435,13 @@
         <v/>
       </c>
       <c r="S1" s="1" t="str">
-        <v/>
+        <v>SSP Fund</v>
       </c>
       <c r="T1" s="1" t="str">
-        <v/>
+        <v>5,000.00</v>
       </c>
       <c r="U1" s="1" t="str">
-        <v/>
+        <v>5,000.00</v>
       </c>
       <c r="V1" s="1" t="str">
         <v/>
@@ -450,13 +450,13 @@
         <v/>
       </c>
       <c r="X1" s="1" t="str">
-        <v/>
+        <v>6,000.00</v>
       </c>
       <c r="Y1" s="1" t="str">
         <v/>
       </c>
       <c r="Z1" s="1" t="str">
-        <v/>
+        <v>6,000.00</v>
       </c>
       <c r="AA1" s="1" t="str">
         <v/>
@@ -465,7 +465,7 @@
         <v/>
       </c>
       <c r="AC1" s="1" t="str">
-        <v/>
+        <v>08 Mar -17</v>
       </c>
       <c r="AD1" s="1" t="str">
         <v/>
@@ -497,7 +497,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="str">
-        <v/>
+        <v>21324</v>
       </c>
       <c r="B2" s="1" t="str">
         <v/>
@@ -506,7 +506,7 @@
         <v/>
       </c>
       <c r="D2" s="1" t="str">
-        <v>NOW</v>
+        <v>TEST</v>
       </c>
       <c r="E2" s="1" t="str">
         <v/>
@@ -551,7 +551,7 @@
         <v/>
       </c>
       <c r="S2" s="1" t="str">
-        <v/>
+        <v>GAA Fund</v>
       </c>
       <c r="T2" s="1" t="str">
         <v/>
@@ -566,10 +566,10 @@
         <v/>
       </c>
       <c r="X2" s="1" t="str">
-        <v>500.00</v>
+        <v/>
       </c>
       <c r="Y2" s="1" t="str">
-        <v>500.00</v>
+        <v/>
       </c>
       <c r="Z2" s="1" t="str">
         <v/>
@@ -581,7 +581,7 @@
         <v/>
       </c>
       <c r="AC2" s="1" t="str">
-        <v>08 Jul -17</v>
+        <v/>
       </c>
       <c r="AD2" s="1" t="str">
         <v/>
@@ -609,122 +609,6 @@
       </c>
       <c r="AL2" s="1" t="str">
         <v/>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="B3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="C3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="D3" s="1" t="str">
-        <v>YEAH</v>
-      </c>
-      <c r="E3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="F3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="G3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="H3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="I3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="J3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="K3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="L3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="M3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="N3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="O3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="P3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="Q3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="R3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="S3" s="1" t="str">
-        <v>SSP Fund</v>
-      </c>
-      <c r="T3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="U3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="V3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="W3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="X3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="Y3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="Z3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AA3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AB3" s="1" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="AC3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AD3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AE3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AF3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AG3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AH3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AI3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AJ3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AK3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="AL3" s="1" t="str">
-        <v xml:space="preserve">  </v>
       </c>
     </row>
   </sheetData>

</xml_diff>